<commit_message>
correction doc v1 04-10-2016
</commit_message>
<xml_diff>
--- a/Doc_SCRUM/LesSprints.xlsx
+++ b/Doc_SCRUM/LesSprints.xlsx
@@ -5,19 +5,19 @@
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-15" windowWidth="10815" windowHeight="12255" activeTab="1"/>
-    <workbookView xWindow="10785" yWindow="-15" windowWidth="14430" windowHeight="12255"/>
+    <workbookView xWindow="10785" yWindow="-15" windowWidth="14430" windowHeight="12255" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tout" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint" sheetId="2" r:id="rId2"/>
-    <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
+    <sheet name="SprntsReview" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="49">
   <si>
     <t xml:space="preserve">Story Name </t>
   </si>
@@ -115,9 +115,6 @@
     <t>congé</t>
   </si>
   <si>
-    <t>Doc technique</t>
-  </si>
-  <si>
     <t>User Case</t>
   </si>
   <si>
@@ -137,6 +134,36 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>Doc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprint 1 </t>
+  </si>
+  <si>
+    <t>Récapitulatif Sprints</t>
+  </si>
+  <si>
+    <t>Jessica</t>
+  </si>
+  <si>
+    <t>Problème</t>
+  </si>
+  <si>
+    <t>Solution</t>
+  </si>
+  <si>
+    <t>Ordinateur(Ralenticement)</t>
+  </si>
+  <si>
+    <t>Réinitialisation de l'ordinateur</t>
+  </si>
+  <si>
+    <t>non</t>
+  </si>
+  <si>
+    <t>Sprint 2</t>
   </si>
 </sst>
 </file>
@@ -194,7 +221,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -399,11 +426,97 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -467,6 +580,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -773,8 +895,8 @@
     <sheetView workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,7 +977,7 @@
         <v>29</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E2" s="20">
         <v>1000</v>
@@ -928,7 +1050,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" s="22" t="s">
         <v>12</v>
@@ -1033,7 +1155,7 @@
         <v>20</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E7" s="18"/>
       <c r="F7" s="18"/>
@@ -1170,9 +1292,7 @@
       <c r="A12" s="22">
         <v>11</v>
       </c>
-      <c r="B12" s="22" t="s">
-        <v>32</v>
-      </c>
+      <c r="B12" s="22"/>
       <c r="C12" s="22" t="s">
         <v>20</v>
       </c>
@@ -1199,7 +1319,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13" s="18" t="s">
         <v>20</v>
@@ -1229,7 +1349,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="22" t="s">
         <v>20</v>
@@ -1257,7 +1377,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="52" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" s="52" t="s">
         <v>20</v>
@@ -1285,7 +1405,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" s="51" t="s">
         <v>20</v>
@@ -1313,7 +1433,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C17" s="49" t="s">
         <v>20</v>
@@ -1594,7 +1714,9 @@
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1664,7 +1786,7 @@
         <v>29</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F4" s="29">
         <v>1000</v>
@@ -1799,9 +1921,6 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="49"/>
       <c r="H9" s="12" t="s">
         <v>25</v>
       </c>
@@ -1860,13 +1979,17 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="27"/>
-      <c r="C14" s="25"/>
+      <c r="C14" s="25" t="s">
+        <v>39</v>
+      </c>
       <c r="D14" s="45" t="s">
         <v>20</v>
       </c>
       <c r="E14" s="25"/>
       <c r="F14" s="29"/>
-      <c r="G14" s="30"/>
+      <c r="G14" s="30">
+        <v>10</v>
+      </c>
       <c r="I14" s="36">
         <v>0</v>
       </c>
@@ -1888,12 +2011,14 @@
         <v>20</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F15" s="7">
         <v>110</v>
       </c>
-      <c r="G15" s="6"/>
+      <c r="G15" s="6">
+        <v>10</v>
+      </c>
       <c r="I15" s="4">
         <v>0</v>
       </c>
@@ -1920,7 +2045,9 @@
       <c r="F16" s="25">
         <v>100</v>
       </c>
-      <c r="G16" s="30"/>
+      <c r="G16" s="30">
+        <v>10</v>
+      </c>
       <c r="I16" s="27">
         <v>0</v>
       </c>
@@ -1936,7 +2063,7 @@
         <v>12</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D17" s="46" t="s">
         <v>20</v>
@@ -1947,7 +2074,9 @@
       <c r="F17" s="5">
         <v>100</v>
       </c>
-      <c r="G17" s="6"/>
+      <c r="G17" s="6">
+        <v>10</v>
+      </c>
       <c r="I17" s="4">
         <v>0</v>
       </c>
@@ -1986,7 +2115,7 @@
     <row r="20" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H20" s="38">
         <f>SUM(G14:G18)</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="I20" s="39">
         <f>SUM(I14:K18)</f>
@@ -2001,13 +2130,130 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="55"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="56"/>
+      <c r="C4" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="60" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="61" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="53" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="57" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="58"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="53" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="54"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="55"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="56"/>
+      <c r="C10" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="60" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="61" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="53" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="57" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="57"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="58"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ajout du Stand Up dans le fichier LesSprints.xlsx
</commit_message>
<xml_diff>
--- a/Doc_SCRUM/LesSprints.xlsx
+++ b/Doc_SCRUM/LesSprints.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="15195" yWindow="-15" windowWidth="9795" windowHeight="12075" activeTab="2"/>
+    <workbookView xWindow="15195" yWindow="-15" windowWidth="9795" windowHeight="12075" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Tout" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint" sheetId="2" r:id="rId2"/>
     <sheet name="SprntsReview" sheetId="3" r:id="rId3"/>
+    <sheet name="stand up " sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="63">
   <si>
     <t xml:space="preserve">Story Name </t>
   </si>
@@ -181,6 +182,30 @@
   </si>
   <si>
     <t>ab</t>
+  </si>
+  <si>
+    <t>ab(dernière heure)</t>
+  </si>
+  <si>
+    <t>gitHub</t>
+  </si>
+  <si>
+    <t>Git extensions (Changement pour des raisons de simplification)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ce que j'ai fait la semaine dernière </t>
+  </si>
+  <si>
+    <t>ce que je vais faire</t>
+  </si>
+  <si>
+    <t>intergration Musique / Son</t>
+  </si>
+  <si>
+    <t>Clique droit Drapeau</t>
+  </si>
+  <si>
+    <t>GitHub possait problème chez Jessica et chez Dilan, donc Mme Travnjak nous a dit de passé à Git Extensions</t>
   </si>
 </sst>
 </file>
@@ -526,7 +551,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -620,6 +645,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -924,8 +952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1751,8 +1779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2311,17 +2339,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="3" max="4" width="58.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -2483,6 +2511,152 @@
       <c r="E18" s="49"/>
       <c r="F18" s="49"/>
     </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="55"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="56"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="50"/>
+      <c r="C21" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="52" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="53" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="F22" s="54" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:F8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5:F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="41.42578125" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" customWidth="1"/>
+    <col min="6" max="6" width="58.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="57">
+        <v>42676</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="70" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="70" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="70" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" s="70" t="s">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>